<commit_message>
Planned EDA for first four fields.
</commit_message>
<xml_diff>
--- a/EDA/eda_planning.xlsx
+++ b/EDA/eda_planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a0l05iw\Documents\toy\house_prices\EDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1683CA0C-51DE-411A-904F-13CC8E940009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5B089A-6ABB-4A92-A28A-AE517A7D67DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_description" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="605">
   <si>
     <t>fields</t>
   </si>
@@ -1841,6 +1841,15 @@
   </si>
   <si>
     <t>Target EDA</t>
+  </si>
+  <si>
+    <t>Boxplot by class / heatmap of mct</t>
+  </si>
+  <si>
+    <t>Histogram</t>
+  </si>
+  <si>
+    <t>Scatterplot</t>
   </si>
 </sst>
 </file>
@@ -2245,8 +2254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE888919-F0FA-4BA8-A542-B191DC88A8EE}">
   <dimension ref="A1:B524"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6459,8 +6468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CF82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6735,21 +6744,41 @@
       <c r="B3" t="s">
         <v>600</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>602</v>
+      </c>
     </row>
     <row r="4" spans="1:84" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>600</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>602</v>
+      </c>
     </row>
     <row r="5" spans="1:84" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>603</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>604</v>
+      </c>
     </row>
     <row r="6" spans="1:84" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>603</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>604</v>
       </c>
     </row>
     <row r="7" spans="1:84" x14ac:dyDescent="0.3">

</xml_diff>